<commit_message>
Auto-committed on 2023/04/06 週四  9:52:13.34
</commit_message>
<xml_diff>
--- a/Program/Other/L9731_底稿_人工檢核表4.xlsx
+++ b/Program/Other/L9731_底稿_人工檢核表4.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>戶號</t>
   </si>
@@ -107,6 +107,14 @@
   </si>
   <si>
     <t>擔保品地區別地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>案件隸屬單位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>企金別</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1153,13 +1161,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1181,9 +1189,10 @@
     <col min="22" max="22" width="11.7265625" customWidth="1"/>
     <col min="23" max="23" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -1257,8 +1266,14 @@
       <c r="X1" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="Y1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="E10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/05 週四 11:55:26.05
</commit_message>
<xml_diff>
--- a/Program/Other/L9731_底稿_人工檢核表4.xlsx
+++ b/Program/Other/L9731_底稿_人工檢核表4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62364E-2FB4-41A7-B16D-D56C08C2BED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F372606-E6A2-4FAA-A159-88F0FECECD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="5670" windowWidth="16840" windowHeight="7740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="放款餘額明細表" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>戶號</t>
   </si>
@@ -127,6 +127,14 @@
   </si>
   <si>
     <t>無擔保資產分類</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利害關係人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特定資產記號</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1173,42 +1181,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE4" sqref="AE4"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17" style="14" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="20.77734375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.77734375" customWidth="1"/>
-    <col min="23" max="23" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.90625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="20.81640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.81640625" customWidth="1"/>
+    <col min="23" max="23" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" customWidth="1"/>
+    <col min="31" max="31" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -1292,19 +1302,25 @@
         <v>25</v>
       </c>
       <c r="AB1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
       <c r="E10"/>
     </row>
   </sheetData>

</xml_diff>